<commit_message>
Worked out a basic OO structure for motors and step generators
</commit_message>
<xml_diff>
--- a/Documents/Clock Calculator.xlsx
+++ b/Documents/Clock Calculator.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Arduino UNO System Clock</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t>Steps/Sec</t>
+  </si>
+  <si>
+    <t>steps/sec</t>
+  </si>
+  <si>
+    <t>IRQ frequency</t>
+  </si>
+  <si>
+    <t>Target step rate</t>
+  </si>
+  <si>
+    <t>Timer 1 OCR1A value</t>
   </si>
 </sst>
 </file>
@@ -196,7 +208,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{45FBD8AE-DBF4-4521-BE95-55E05CED37C1}" name="Table1" displayName="Table1" ref="A2:I12" totalsRowShown="0" headerRowDxfId="1" headerRowCellStyle="Heading 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{45FBD8AE-DBF4-4521-BE95-55E05CED37C1}" name="Table1" displayName="Table1" ref="A2:I12" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A2:I12" xr:uid="{A2FCEC19-4309-4A23-8523-65993E2F5669}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{6055C051-1489-40A3-AE62-818D17B5087A}" name="Column1"/>
@@ -512,16 +524,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB4AA852-18F9-4D42-9022-5EDE437C363C}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
@@ -875,10 +888,43 @@
         <v>13333.333333333334</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>1000</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <f>B15*2</f>
+        <v>2000</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <f>E10/B16</f>
+        <v>8000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>